<commit_message>
Map city stats & sms
</commit_message>
<xml_diff>
--- a/SMS/SMS_data.xlsx
+++ b/SMS/SMS_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>ΠΡΟΛΑΒΕ ΤΗΝ 1+1 ΠΡΟΣΦΟΡΑ! ΜΕΧΡΙ ΤΗΝ ΚΥΡΙΑΚΗ 8/2 ΜΕ ΚΑΘΕ Goody's Extreme Burger Η CLICKDELIVERY ΣΟΥ ΚΑΝΕΙ ΔΩΡΟ ΑΛΛΟ ΕΝΑ! ΠΑΡΑΓΓΕΙΛΕ ΤΩΡΑ ΣΤΟ www.clickdelivery.gr</t>
+  </si>
+  <si>
+    <t>ΠΡΟΛΑΒΕ ΤΗΝ 1+1 ΠΡΟΣΦΟΡΑ:ΜΕΧΡΙ ΤΗΝ ΚΥΡΙΑΚΗ 15/3 ΜΕ ΚΑΘΕ Goody's Extreme Burger Η CLICKDELIVERY ΣΟΥ ΚΑΝΕΙ ΔΩΡΟ ΑΛΛΟ ΕΝΑ! ΠΑΡΑΓΓΕΙΛΕ ΤΩΡΑ ΣΤΟ www.clickdelivery.gr</t>
   </si>
 </sst>
 </file>
@@ -70,10 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,7 +383,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +438,7 @@
         <v>15368</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="0">+LEN(C3)</f>
+        <f t="shared" ref="E3:E9" si="0">+LEN(C3)</f>
         <v>160</v>
       </c>
     </row>
@@ -534,8 +536,19 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="1">
+        <v>42074</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>23934</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>